<commit_message>
Just for recording: for DynamicClause definitions.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoDbCommonConstants.xlsx
+++ b/meta/program/BlancoDbCommonConstants.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbCommon/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BB63F507-D6AA-4F4F-A4AC-5AE68A9FD8B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F26044-5E75-8945-BB50-B2BEDA2BCE74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="64000" windowHeight="21140" tabRatio="640"/>
+    <workbookView xWindow="28660" yWindow="4300" windowWidth="19260" windowHeight="19680" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -34,14 +34,6 @@
     <definedName name="必須">#REF!</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -162,14 +154,14 @@
     <t>○</t>
   </si>
   <si>
-    <t>"2.1.0."</t>
+    <t>"2.1.1."</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -952,7 +944,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1325,19 +1317,19 @@
   </mergeCells>
   <phoneticPr fontId="4"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D47" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>adjustConstValue</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>isAbstract</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>accessScope</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1351,7 +1343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
[POI4] 2.2.0: Now ready to use apache poi 4.1.2.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoDbCommonConstants.xlsx
+++ b/meta/program/BlancoDbCommonConstants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbCommon/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F26044-5E75-8945-BB50-B2BEDA2BCE74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB029D4F-FFF5-A647-8248-EF27167621B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28660" yWindow="4300" windowWidth="19260" windowHeight="19680" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19140" yWindow="1920" windowWidth="19260" windowHeight="19680" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="constants" sheetId="1" r:id="rId1"/>
@@ -154,7 +154,7 @@
     <t>○</t>
   </si>
   <si>
-    <t>"2.1.1."</t>
+    <t>"2.2.0"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>

</xml_diff>

<commit_message>
3.0.3: Enable using FUNCTION_TAG in targetItem for IN, NOT IN, BETWEEN, NOT BETWEEN condition type.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoDbCommonConstants.xlsx
+++ b/meta/program/BlancoDbCommonConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbCommon/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB029D4F-FFF5-A647-8248-EF27167621B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBF0263-5CFD-BB4A-B14A-26A6F0F078A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19140" yWindow="1920" windowWidth="19260" windowHeight="19680" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,7 +154,7 @@
     <t>○</t>
   </si>
   <si>
-    <t>"2.2.0"</t>
+    <t>"3.0.3"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -500,29 +500,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -583,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
@@ -592,16 +591,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -625,9 +624,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -665,9 +664,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -700,26 +699,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -752,26 +734,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1033,43 +998,43 @@
         <v>12</v>
       </c>
       <c r="D9"/>
-      <c r="E9" s="15"/>
+      <c r="E9"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="16"/>
+      <c r="C10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="D10"/>
+      <c r="E10"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="D11"/>
+      <c r="E11"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12"/>
+      <c r="E12"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
@@ -1081,13 +1046,13 @@
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="7"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16"/>
@@ -1101,201 +1066,201 @@
       <c r="A17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="7"/>
       <c r="G17"/>
       <c r="H17"/>
     </row>
     <row r="18" spans="1:8" ht="13.5" customHeight="1">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="22"/>
+      <c r="F18" s="21"/>
       <c r="G18"/>
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="45"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="23"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="22"/>
       <c r="G19"/>
       <c r="H19"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="24">
+      <c r="A20" s="23">
         <v>1</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="28"/>
+      <c r="F20" s="27"/>
       <c r="G20"/>
       <c r="H20"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="24">
+      <c r="A21" s="23">
         <v>2</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="30"/>
+      <c r="F21" s="29"/>
       <c r="G21"/>
       <c r="H21"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="24">
+      <c r="A22" s="23">
         <v>3</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="30"/>
+      <c r="F22" s="29"/>
       <c r="G22"/>
       <c r="H22"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="24">
+      <c r="A23" s="23">
         <v>4</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="30"/>
+      <c r="F23" s="29"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="24"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="30"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="29"/>
       <c r="G24"/>
       <c r="H24"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="30"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="29"/>
       <c r="G25"/>
       <c r="H25"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="30"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="29"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="30"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="29"/>
       <c r="G27"/>
       <c r="H27"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="31"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="33"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
       <c r="G28"/>
       <c r="H28"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="31"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
+      <c r="A29" s="30"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
       <c r="G29"/>
       <c r="H29"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="31"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
+      <c r="A30" s="30"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
       <c r="G30"/>
       <c r="H30"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="34"/>
-      <c r="B31" s="35"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="37"/>
+      <c r="A31" s="33"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="36"/>
       <c r="G31"/>
       <c r="H31"/>
     </row>
@@ -1378,34 +1343,34 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="37" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="39"/>
-      <c r="D4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="B4" s="38"/>
+      <c r="D4" s="39"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="41" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="43"/>
+      <c r="B6" s="42"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>

</xml_diff>

<commit_message>
3.0.4 to add options addIntrospected : add introspected annotation to Row class. noFinalize: finalize method is deprecated from Java 9.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoDbCommonConstants.xlsx
+++ b/meta/program/BlancoDbCommonConstants.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoDbCommon/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBF0263-5CFD-BB4A-B14A-26A6F0F078A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E082F0-F83A-FD42-9BD2-109B76FBD775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19140" yWindow="1920" windowWidth="19260" windowHeight="19680" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,7 +154,7 @@
     <t>○</t>
   </si>
   <si>
-    <t>"3.0.3"</t>
+    <t>"3.0.4"</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>

</xml_diff>